<commit_message>
Add more universities to dummy data and update templates with 8 sample records
</commit_message>
<xml_diff>
--- a/source_code/templates/peserta_upload_template.xlsx
+++ b/source_code/templates/peserta_upload_template.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -595,6 +595,87 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>P006</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Rina Sari</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>UNIV04</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>rina.sari@univ4.edu</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>081678901234</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>P007</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Andi Wijaya</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>UNIV05</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>andi.wijaya@univ5.edu</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>081789012345</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>P008</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Lisa Putri</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>UNIV06</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>lisa.putri@univ6.edu</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>081890123456</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>